<commit_message>
Solucionando problema con los UpLoad de archivos
Se coluciona problema con el UpLoaading de archivos  para los modulos de wingman y para su futuro uso en Compliance.

Se continua con identificacion de elementos.
</commit_message>
<xml_diff>
--- a/KavakoWebBot/KavakoWebBotTools/DataPool/KOS_Wingman.xlsx
+++ b/KavakoWebBot/KavakoWebBotTools/DataPool/KOS_Wingman.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSUE-CRUZ\source\repos\KavakoWebBot\KavakoWebBotTools\DataPool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSUE-CRUZ\Documents\GitHub\KavakQA\KavakoWebBot\KavakoWebBotTools\DataPool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3790AB50-4EAC-44A2-8CD2-B749D2BDEB3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC19E1-99EA-4A2D-BCA9-00DA1AC6CBA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6540" yWindow="2910" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="167">
   <si>
     <t>ResultadoEsperado</t>
   </si>
@@ -527,6 +527,9 @@
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>C:\Users\JOSUE-CRUZ\Downloads\Kavak.png</t>
   </si>
 </sst>
 </file>
@@ -967,59 +970,59 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1569,7 +1572,7 @@
       <c r="XEV3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="XEW3" s="41" t="s">
+      <c r="XEW3" s="57" t="s">
         <v>19</v>
       </c>
       <c r="XEX3" s="1" t="s">
@@ -1639,7 +1642,7 @@
       <c r="XEV4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="XEW4" s="42"/>
+      <c r="XEW4" s="58"/>
       <c r="XEX4" s="1"/>
       <c r="XEY4" s="1"/>
       <c r="XEZ4" s="3" t="s">
@@ -1660,7 +1663,7 @@
       <c r="XEV5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="XEW5" s="41" t="s">
+      <c r="XEW5" s="57" t="s">
         <v>134</v>
       </c>
       <c r="XEX5" s="1"/>
@@ -1681,7 +1684,7 @@
       <c r="XEV6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="XEW6" s="42"/>
+      <c r="XEW6" s="58"/>
       <c r="XEX6" s="1"/>
       <c r="XEY6" s="1"/>
       <c r="XEZ6" s="3" t="s">
@@ -1886,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AF6" sqref="AF6"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2136,7 @@
         <v>165</v>
       </c>
       <c r="V2" s="24" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="W2" s="25" t="s">
         <v>55</v>
@@ -2248,7 +2251,7 @@
         <v>165</v>
       </c>
       <c r="V3" s="17" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="W3" s="15" t="s">
         <v>55</v>
@@ -2317,116 +2320,116 @@
       </c>
     </row>
     <row r="4" spans="1:38 16378:16383" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="48" t="s">
+      <c r="D4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="46">
         <v>5544332200</v>
       </c>
-      <c r="I4" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="48" t="s">
+      <c r="I4" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="48" t="s">
+      <c r="L4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="M4" s="48" t="s">
+      <c r="M4" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="N4" s="48" t="s">
+      <c r="N4" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="P4" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q4" s="48" t="s">
+      <c r="P4" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="R4" s="48" t="s">
+      <c r="R4" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="S4" s="48" t="s">
+      <c r="S4" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="48" t="s">
+      <c r="T4" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="U4" s="48" t="s">
+      <c r="U4" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="V4" s="48" t="s">
+      <c r="V4" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="W4" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y4" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z4" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA4" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB4" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="W4" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="X4" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y4" s="49" t="s">
-        <v>142</v>
-      </c>
-      <c r="Z4" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA4" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB4" s="49" t="s">
+      <c r="AC4" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="AC4" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="AD4" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE4" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF4" s="43" t="str">
+      <c r="AD4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF4" s="41" t="str">
         <f t="shared" si="1"/>
         <v>Norberto Rivera</v>
       </c>
-      <c r="AG4" s="50" t="s">
+      <c r="AG4" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="AH4" s="49" t="s">
+      <c r="AH4" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="AI4" s="50" t="s">
+      <c r="AI4" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="AJ4" s="49" t="s">
+      <c r="AJ4" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="AK4" s="51" t="s">
+      <c r="AK4" s="49" t="s">
         <v>153</v>
       </c>
       <c r="AL4" s="19"/>
@@ -2514,7 +2517,7 @@
         <v>165</v>
       </c>
       <c r="V5" s="24" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="W5" s="27" t="s">
         <v>55</v>
@@ -2537,7 +2540,7 @@
       <c r="AC5" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="AD5" s="57" t="s">
+      <c r="AD5" s="55" t="s">
         <v>54</v>
       </c>
       <c r="AE5" s="23" t="s">
@@ -2647,7 +2650,7 @@
         <v>165</v>
       </c>
       <c r="V6" s="17" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="W6" s="14" t="s">
         <v>55</v>
@@ -2774,7 +2777,7 @@
         <v>165</v>
       </c>
       <c r="V7" s="34" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="W7" s="37" t="s">
         <v>55</v>
@@ -2797,7 +2800,7 @@
       <c r="AC7" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="AD7" s="58" t="s">
+      <c r="AD7" s="56" t="s">
         <v>54</v>
       </c>
       <c r="AE7" s="33" t="s">
@@ -2837,116 +2840,116 @@
       </c>
     </row>
     <row r="8" spans="1:38 16378:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="55" t="s">
+      <c r="D8" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="55" t="s">
+      <c r="G8" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="55">
+      <c r="H8" s="53">
         <v>5544332200</v>
       </c>
-      <c r="I8" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" s="55" t="s">
+      <c r="I8" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="55" t="s">
+      <c r="K8" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="55" t="s">
+      <c r="L8" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="M8" s="55" t="s">
+      <c r="M8" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="55" t="s">
+      <c r="N8" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="O8" s="55" t="s">
+      <c r="O8" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="P8" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q8" s="55" t="s">
+      <c r="P8" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="R8" s="55" t="s">
+      <c r="R8" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="S8" s="55" t="s">
+      <c r="S8" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="T8" s="55" t="s">
+      <c r="T8" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="U8" s="55" t="s">
+      <c r="U8" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="V8" s="55" t="s">
+      <c r="V8" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="W8" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="X8" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y8" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z8" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA8" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB8" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="W8" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="X8" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y8" s="55" t="s">
-        <v>142</v>
-      </c>
-      <c r="Z8" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA8" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB8" s="55" t="s">
+      <c r="AC8" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="AC8" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AD8" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE8" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF8" s="44" t="str">
+      <c r="AD8" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE8" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF8" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Norberto Rivera</v>
       </c>
-      <c r="AG8" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH8" s="55" t="s">
+      <c r="AG8" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="AI8" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ8" s="55" t="s">
+      <c r="AI8" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ8" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="AK8" s="56" t="s">
+      <c r="AK8" s="54" t="s">
         <v>153</v>
       </c>
       <c r="AL8" s="19"/>
@@ -3028,7 +3031,7 @@
         <v>165</v>
       </c>
       <c r="V9" s="17" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="W9" s="16" t="s">
         <v>55</v>
@@ -3155,7 +3158,7 @@
         <v>165</v>
       </c>
       <c r="V10" s="34" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
       <c r="W10" s="33" t="s">
         <v>55</v>

</xml_diff>